<commit_message>
added all thing to diss
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndrewM\Documents\GitHub\Honours\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CAE34D0-8BB6-4A26-9611-E15A3209931C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DA21FD0-F0D8-47B9-AD10-E3CE14F3D3CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1350" windowWidth="20490" windowHeight="7680" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2700" windowWidth="20490" windowHeight="7680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form responses 1" sheetId="1" r:id="rId1"/>
@@ -582,9 +582,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Form responses 1'!$E$21:$E$26</c:f>
+              <c:f>'Form responses 1'!$E$21:$E$27</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>Happy</c:v>
                 </c:pt>
@@ -602,33 +602,39 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>Boring</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Other</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Form responses 1'!$F$21:$F$26</c:f>
+              <c:f>'Form responses 1'!$G$21:$G$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.3888888888888889</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.22222222222222221</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.5555555555555552E-2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.1111111111111111</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.1111111111111111</c:v>
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3312,18 +3318,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$5:$H$7</c:f>
+              <c:f>Sheet1!$G$5:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>41.358024691358025</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24.691358024691358</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>33.950617283950621</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3990,21 +3996,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Form responses 1'!$H$21:$H$26</c:f>
+              <c:f>'Form responses 1'!$I$21:$I$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>5.5555555555555552E-2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.61111111111111116</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.22222222222222221</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -8379,7 +8385,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Form responses 1'!$J$21:$J$27</c:f>
+              <c:f>'Form responses 1'!$K$21:$K$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -8390,19 +8396,19 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.1875</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.6875</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.25E-2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.25E-2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12741,7 +12747,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Form responses 1'!$M$21:$M$26</c:f>
+              <c:f>'Form responses 1'!$N$21:$N$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -12752,10 +12758,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.29411764705882354</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.70588235294117652</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -42613,15 +42619,15 @@
   </sheetPr>
   <dimension ref="A1:AI32"/>
   <sheetViews>
-    <sheetView topLeftCell="X1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AD17" sqref="AD17"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="16" width="21.5703125" customWidth="1"/>
-    <col min="17" max="17" width="29" customWidth="1"/>
+    <col min="17" max="17" width="53.85546875" customWidth="1"/>
     <col min="18" max="47" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -44449,8 +44455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF9F32CB-DB16-4F07-A090-2A107F06B04F}">
   <dimension ref="A1:S24"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+    <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -45907,8 +45913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6315E4DB-183B-4987-872E-BC707019C387}">
   <dimension ref="A1:AF24"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -47436,10 +47442,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A2213EF-0955-415D-B36E-0268747D0EB2}">
   <dimension ref="A1:AF27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="Z1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="AA1" sqref="AA1"/>
-      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
+      <selection pane="bottomLeft" activeCell="AI13" sqref="AI13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -49114,8 +49120,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58F5CF14-153A-4FE1-86B8-6AA34D879E40}">
   <dimension ref="A1:AE19"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+    <sheetView topLeftCell="T1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AD2" sqref="AD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>